<commit_message>
Get simpleImportComplexMetadata test to pass
* Update metadata namespace in the worksheet to the new namespace. The outdated namespace was the sole cause of the subtle and difficult-to-debug test failure.
</commit_message>
<xml_diff>
--- a/src/integration-test/resources/simpleImportComplexMetadata.xlsx
+++ b/src/integration-test/resources/simpleImportComplexMetadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/code/metadata-catalogue/mc-plugins/mc-plugin-excel/src/integration-test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjl/code/maurodatamapper-plugins/mdm-plugin-excel/src/integration-test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D3E4DE-7CDB-0548-A480-25770703F32C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75647DC-4E80-8346-A111-B4EAA8035D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
+    <workbookView xWindow="17920" yWindow="460" windowWidth="17920" windowHeight="20280" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="DataModels" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>ox.softeng.metadatacatalogue.plugins.excel</t>
+    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel</t>
   </si>
 </sst>
 </file>
@@ -494,50 +494,50 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CEC267-E7D6-814F-BC88-B2D73C8A9138}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,10 +868,11 @@
     <col min="6" max="6" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="26.5" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="30" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
@@ -890,10 +891,10 @@
       <c r="F1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="12"/>
       <c r="J1" s="7" t="s">
         <v>68</v>
@@ -906,7 +907,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="20"/>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="15" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="13" t="s">
@@ -953,13 +954,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F50" xr:uid="{0AF974D4-8E76-DB43-B4D3-3BE4F426655A}">
@@ -1008,10 +1009,10 @@
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -1020,13 +1021,13 @@
       <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="29" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="10" t="s">
@@ -1035,11 +1036,11 @@
       <c r="L1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
       <c r="P1" s="10" t="s">
         <v>70</v>
       </c>
@@ -1052,13 +1053,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11" t="s">
@@ -1187,57 +1188,57 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="23">
         <v>0</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="23">
         <v>-1</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="23"/>
       <c r="I8" t="s">
         <v>39</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
       <c r="I9" t="s">
         <v>41</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B10" t="s">
@@ -1264,29 +1265,29 @@
       <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="22" t="s">
+      <c r="O10" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="22"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="22"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1373,6 +1374,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A10:A12"/>
@@ -1385,11 +1391,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="D3:E8 D10:E50" xr:uid="{E117BD47-683C-E64F-9082-625073EC8D0C}">

</xml_diff>